<commit_message>
添加 training_type 和 subject_code 的词典映射
</commit_message>
<xml_diff>
--- a/excel_export_python/export_test_1.xlsx
+++ b/excel_export_python/export_test_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>410067</t>
   </si>
@@ -101,6 +101,27 @@
   </si>
   <si>
     <t>12131231231@qq.com</t>
+  </si>
+  <si>
+    <t>试一试</t>
+  </si>
+  <si>
+    <t>410304199312140590</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>13298309877</t>
+  </si>
+  <si>
+    <t>43-2012215-201405598</t>
   </si>
 </sst>
 </file>
@@ -432,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -570,6 +591,47 @@
         <v>25</v>
       </c>
     </row>
+    <row r="4" spans="1:20">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>